<commit_message>
add the updated test case
</commit_message>
<xml_diff>
--- a/ResourcesFolder/TestData.xlsx
+++ b/ResourcesFolder/TestData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="50">
   <si>
     <t>Comment</t>
   </si>
@@ -163,6 +163,9 @@
   </si>
   <si>
     <t>Every week, highest scorer wins additional £50 gift voucher</t>
+  </si>
+  <si>
+    <t>List_banner</t>
   </si>
 </sst>
 </file>
@@ -526,7 +529,7 @@
   <dimension ref="A1:V26"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -536,7 +539,7 @@
     <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="25.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.5703125" customWidth="1"/>
     <col min="7" max="7" width="21.42578125" customWidth="1"/>
     <col min="8" max="8" width="24.140625" customWidth="1"/>
     <col min="11" max="11" width="14.5703125" customWidth="1"/>
@@ -544,6 +547,7 @@
     <col min="13" max="13" width="16.28515625" customWidth="1"/>
     <col min="14" max="14" width="16.42578125" customWidth="1"/>
     <col min="17" max="17" width="15.5703125" customWidth="1"/>
+    <col min="18" max="18" width="18.140625" customWidth="1"/>
     <col min="19" max="19" width="15.140625" customWidth="1"/>
     <col min="20" max="20" width="15.85546875" customWidth="1"/>
     <col min="21" max="21" width="12" customWidth="1"/>
@@ -775,73 +779,95 @@
       <c r="B23" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="C23" s="5" t="s">
+      <c r="C23" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="D23" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="D23" s="5" t="s">
+      <c r="E23" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="E23" s="6" t="s">
+      <c r="F23" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="F23" s="6" t="s">
+      <c r="G23" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="G23" s="6" t="s">
+      <c r="H23" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="H23" s="6" t="s">
+      <c r="I23" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="I23" s="6" t="s">
+      <c r="J23" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="J23" s="6" t="s">
+      <c r="K23" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="K23" s="6" t="s">
+      <c r="L23" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="L23" s="6" t="s">
+      <c r="M23" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="M23" s="6" t="s">
+      <c r="N23" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="N23" s="6" t="s">
+      <c r="O23" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="O23" s="6" t="s">
+      <c r="P23" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="P23" s="6" t="s">
+      <c r="Q23" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="Q23" s="6" t="s">
+      <c r="R23" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="R23" s="6" t="s">
+      <c r="S23" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="S23" s="6" t="s">
+      <c r="T23" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="T23" s="6" t="s">
+      <c r="U23" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="U23" s="6" t="s">
+      <c r="V23" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="V23" s="6"/>
     </row>
     <row r="24" spans="1:22">
       <c r="A24" s="9"/>
       <c r="B24" t="s">
         <v>8</v>
       </c>
+      <c r="C24" s="7"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="6"/>
+      <c r="G24" s="6"/>
+      <c r="H24" s="6"/>
+      <c r="I24" s="6"/>
+      <c r="J24" s="6"/>
+      <c r="K24" s="6"/>
+      <c r="L24" s="6"/>
+      <c r="M24" s="6"/>
+      <c r="N24" s="6"/>
+      <c r="O24" s="6"/>
+      <c r="P24" s="6"/>
+      <c r="Q24" s="6"/>
+      <c r="R24" s="6"/>
+      <c r="S24" s="6"/>
+      <c r="T24" s="6"/>
+      <c r="U24" s="6"/>
+      <c r="V24" s="6"/>
     </row>
     <row r="25" spans="1:22">
-      <c r="A25" s="9" t="s">
+      <c r="A25" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>